<commit_message>
updated power and temp data in exp 6
</commit_message>
<xml_diff>
--- a/experiments/09_power_eval_1/temperatures2.xlsx
+++ b/experiments/09_power_eval_1/temperatures2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_TEMP2\experiment_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E4585B-133B-4A6A-862D-2100C321BFA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947D76F9-3972-4A7C-95A0-21C9C9E9C04E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D9B2736F-8484-4142-882C-94BEA7D2BB42}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="18">
   <si>
     <t>Run 1</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Mod. B Eik LTF</t>
+  </si>
+  <si>
+    <t>Mod.2 B predictor</t>
   </si>
 </sst>
 </file>
@@ -1227,6 +1230,9 @@
               <c:f>'imx8 results'!$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mod.2 B predictor</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1253,10 +1259,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.63734728018212661</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.18861129929625542</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0</c:v>
@@ -1271,10 +1277,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.63734728018212661</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>0.18861129929625542</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0</c:v>
@@ -1320,10 +1326,10 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>58.838666666666661</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>57.372666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2772,6 +2778,9 @@
               <c:f>'imx8 results'!$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mod.2 B predictor</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -2798,10 +2807,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.12811286690518886</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>5.5569855937267987E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0</c:v>
@@ -2816,10 +2825,10 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.12811286690518886</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>5.5569855937267987E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0</c:v>
@@ -2865,10 +2874,10 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>31.788999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>31.526266666666668</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4983,8 +4992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C717F6D4-64AC-45FC-95B6-DC01725ED549}">
   <dimension ref="A35:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5373,41 +5382,55 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="17" t="e">
+      <c r="A44" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="3">
+        <v>59.58</v>
+      </c>
+      <c r="C44" s="3">
+        <v>58.911999999999999</v>
+      </c>
+      <c r="D44" s="3">
+        <v>58.024000000000001</v>
+      </c>
+      <c r="E44" s="17">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F44" s="17" t="e">
+        <v>58.838666666666661</v>
+      </c>
+      <c r="F44" s="17">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.63734728018212661</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31.736599999999999</v>
       </c>
       <c r="H44" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>31.965399999999999</v>
       </c>
       <c r="I44" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>31.664999999999999</v>
       </c>
       <c r="J44" s="17">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>31.788999999999998</v>
       </c>
       <c r="K44" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L44" s="21"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="22"/>
+        <v>0.12811286690518886</v>
+      </c>
+      <c r="L44" s="21">
+        <v>27.843399999999999</v>
+      </c>
+      <c r="M44" s="3">
+        <v>26.9466</v>
+      </c>
+      <c r="N44" s="22">
+        <v>26.359000000000002</v>
+      </c>
     </row>
     <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
@@ -5896,41 +5919,55 @@
       </c>
     </row>
     <row r="58" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="17" t="e">
+      <c r="A58" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="3">
+        <v>57.603999999999999</v>
+      </c>
+      <c r="C58" s="3">
+        <v>57.372</v>
+      </c>
+      <c r="D58" s="3">
+        <v>57.142000000000003</v>
+      </c>
+      <c r="E58" s="17">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F58" s="17" t="e">
+        <v>57.372666666666667</v>
+      </c>
+      <c r="F58" s="17">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.18861129929625542</v>
       </c>
       <c r="G58" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>31.581399999999999</v>
       </c>
       <c r="H58" s="3">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>31.5472</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>31.450200000000002</v>
       </c>
       <c r="J58" s="17">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>31.526266666666668</v>
       </c>
       <c r="K58" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="L58" s="21"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="22"/>
+        <v>5.5569855937267987E-2</v>
+      </c>
+      <c r="L58" s="21">
+        <v>26.022600000000001</v>
+      </c>
+      <c r="M58" s="3">
+        <v>25.8248</v>
+      </c>
+      <c r="N58" s="22">
+        <v>25.691800000000001</v>
+      </c>
     </row>
     <row r="59" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
@@ -6419,7 +6456,9 @@
       </c>
     </row>
     <row r="72" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
+      <c r="A72" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>

</xml_diff>